<commit_message>
changed critical tasks to show the correct length
</commit_message>
<xml_diff>
--- a/2020-10-09_Project-Methodology_ca_Fredrik-Markestad_FP01.xlsx
+++ b/2020-10-09_Project-Methodology_ca_Fredrik-Markestad_FP01.xlsx
@@ -118,12 +118,14 @@
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="10">
     <fill>
@@ -308,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -327,8 +329,8 @@
     <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -342,13 +344,13 @@
     </xf>
     <xf borderId="10" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="11" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -362,12 +364,15 @@
     <xf borderId="10" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="11" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="10" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="10" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -376,10 +381,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="10" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -781,7 +785,7 @@
       <c r="B12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="25">
         <v>3.0</v>
       </c>
       <c r="E12" s="15"/>
@@ -801,33 +805,33 @@
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
-      <c r="G13" s="25"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14">
       <c r="A14" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="22">
         <v>1.0</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="27"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="28"/>
     </row>
     <row r="15">
       <c r="A15" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="22">
         <v>1.0</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="27"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16">
       <c r="A16" s="7"/>
@@ -840,86 +844,85 @@
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="18">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="28"/>
+      <c r="L17" s="29"/>
+      <c r="N17" s="26"/>
     </row>
     <row r="18">
       <c r="A18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="22">
         <v>4.0</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="25"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19">
       <c r="A19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="22">
         <v>3.0</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="25"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="26"/>
     </row>
     <row r="20">
       <c r="A20" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="22">
         <v>3.0</v>
       </c>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21">
       <c r="A21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="22">
         <v>2.0</v>
       </c>
-      <c r="J21" s="32"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
     </row>
     <row r="22">
       <c r="A22" s="20"/>
       <c r="B22" s="16"/>
       <c r="C22" s="17"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
     </row>
     <row r="23">
       <c r="A23" s="12" t="s">
@@ -927,69 +930,68 @@
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="19"/>
+        <v>4.0</v>
+      </c>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="29"/>
     </row>
     <row r="24">
       <c r="A24" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="22">
         <v>2.0</v>
       </c>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="25"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="26"/>
     </row>
     <row r="25">
       <c r="A25" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="22">
         <v>3.0</v>
       </c>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="34"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
     </row>
     <row r="26">
       <c r="A26" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="22">
         <v>2.0</v>
       </c>
-      <c r="K26" s="27"/>
-      <c r="L26" s="33"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
     </row>
     <row r="27">
       <c r="A27" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="22">
         <v>2.0</v>
       </c>
-      <c r="M27" s="36"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="28"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="26"/>
     </row>
     <row r="28">
       <c r="A28" s="7"/>
@@ -1002,7 +1004,7 @@
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="18">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
@@ -1012,37 +1014,36 @@
       <c r="R29" s="15"/>
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="19"/>
+      <c r="U29" s="29"/>
     </row>
     <row r="30">
       <c r="A30" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="22">
         <v>2.0</v>
       </c>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
     </row>
     <row r="31">
       <c r="A31" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="34" t="s">
         <v>26</v>
       </c>
       <c r="C31" s="22">
         <v>5.0</v>
       </c>
-      <c r="Q31" s="37"/>
-      <c r="R31" s="37"/>
-      <c r="S31" s="37"/>
-      <c r="T31" s="37"/>
-      <c r="U31" s="37"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="23"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="35"/>
     </row>
     <row r="32">
       <c r="A32" s="7"/>
@@ -1054,18 +1055,18 @@
         <v>27</v>
       </c>
       <c r="B33" s="13"/>
-      <c r="C33" s="18">
+      <c r="C33" s="25">
         <v>5.0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="40">
+      <c r="C34" s="38">
         <v>5.0</v>
       </c>
     </row>

</xml_diff>